<commit_message>
Upload latest bulk uploader:Change Zaya PFee
</commit_message>
<xml_diff>
--- a/resources/documents/bulk_uploader.xlsx
+++ b/resources/documents/bulk_uploader.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\azsantos\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB4561B6-8941-4858-97AA-6392FAC6B87D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EC13740-129B-4EC0-9B98-793397D66891}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" xr2:uid="{7C7D23D3-7ADE-4CAA-BE9F-CBA28F8BCF2C}"/>
   </bookViews>
@@ -955,8 +955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CC6F7D0-AE9E-4955-9E40-B625F709BCBF}">
   <dimension ref="A1:AO17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Z22" sqref="Z22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2176,7 +2176,7 @@
         <v>1</v>
       </c>
       <c r="X12" s="23">
-        <v>2000</v>
+        <v>10000</v>
       </c>
       <c r="Y12" s="15" t="s">
         <v>43</v>
@@ -2275,7 +2275,7 @@
         <v>1</v>
       </c>
       <c r="X13" s="23">
-        <v>2000</v>
+        <v>10000</v>
       </c>
       <c r="Y13" s="15" t="s">
         <v>43</v>
@@ -2374,7 +2374,7 @@
         <v>1</v>
       </c>
       <c r="X14" s="23">
-        <v>2000</v>
+        <v>10000</v>
       </c>
       <c r="Y14" s="15" t="s">
         <v>43</v>
@@ -2473,7 +2473,7 @@
         <v>1</v>
       </c>
       <c r="X15" s="23">
-        <v>2000</v>
+        <v>10000</v>
       </c>
       <c r="Y15" s="15" t="s">
         <v>43</v>
@@ -2570,7 +2570,7 @@
         <v>1</v>
       </c>
       <c r="X16" s="23">
-        <v>2000</v>
+        <v>10000</v>
       </c>
       <c r="Y16" s="15" t="s">
         <v>43</v>
@@ -2669,7 +2669,7 @@
         <v>1</v>
       </c>
       <c r="X17" s="23">
-        <v>2000</v>
+        <v>10000</v>
       </c>
       <c r="Y17" s="15" t="s">
         <v>43</v>
@@ -2908,7 +2908,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF80F4B0-1A0C-4F20-AD74-B6C9911C45E7}">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>

</xml_diff>